<commit_message>
plan to mod user db
</commit_message>
<xml_diff>
--- a/db/prosess.xlsx
+++ b/db/prosess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A1A8ED-4249-47D2-B0F4-4670FD659DA4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6592C892-D64D-4333-8566-8C9198CF3C28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11130" yWindow="1905" windowWidth="17055" windowHeight="12465" xr2:uid="{9A5316F9-547A-4D45-8B79-A41DABB2FF9A}"/>
+    <workbookView xWindow="6600" yWindow="2340" windowWidth="21600" windowHeight="11505" xr2:uid="{9A5316F9-547A-4D45-8B79-A41DABB2FF9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,10 +80,6 @@
   </si>
   <si>
     <t>修改时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>禁用标志</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -459,7 +455,7 @@
   <dimension ref="C1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -487,7 +483,7 @@
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.2">
@@ -513,17 +509,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="I8" t="s">
-        <v>14</v>
-      </c>
-    </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="I9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.2">

</xml_diff>